<commit_message>
Cleaned up files: 1.2
</commit_message>
<xml_diff>
--- a/EntranceInfo.xlsx
+++ b/EntranceInfo.xlsx
@@ -401,7 +401,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q9" sqref="Q9"/>
@@ -681,6 +681,51 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>45171</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>23:15</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>23:15</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Test</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>User</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>test@test.com</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Galipatia</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Sophomore</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>